<commit_message>
Added columns for the future
</commit_message>
<xml_diff>
--- a/Spreadsheet_with_words.xlsx
+++ b/Spreadsheet_with_words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valdemar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78C7770C-81B6-45FC-BD15-BA281D6D61A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523E9978-C3B9-4B60-A97B-E93A1EA01C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5880" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{9E87C3E0-E587-44D3-9044-F8A174CA6613}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Adjectives</t>
   </si>
@@ -172,6 +172,18 @@
   </si>
   <si>
     <t>Swimming</t>
+  </si>
+  <si>
+    <t>User_words</t>
+  </si>
+  <si>
+    <t>Banned words</t>
+  </si>
+  <si>
+    <t>Hitler</t>
+  </si>
+  <si>
+    <t>Nazi</t>
   </si>
 </sst>
 </file>
@@ -523,15 +535,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD4C108-5E84-4403-864A-02BA902363EF}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -541,8 +553,14 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -552,8 +570,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -563,8 +584,11 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -575,7 +599,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -586,7 +610,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -597,7 +621,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -608,7 +632,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -619,7 +643,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -630,7 +654,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -641,7 +665,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -652,7 +676,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -660,7 +684,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -668,7 +692,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>41</v>
       </c>
@@ -676,7 +700,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>15</v>
       </c>
@@ -684,7 +708,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>16</v>
       </c>

</xml_diff>